<commit_message>
Fix all file tests
</commit_message>
<xml_diff>
--- a/src/test/resources/files/asset_category.xlsx
+++ b/src/test/resources/files/asset_category.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\labs\monoliths\fixed-assets\src\test\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC2E036-32A7-4BC6-BEF3-43417AA49EDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847EF646-E3C8-428F-96F0-9888B00F756F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="885" yWindow="-120" windowWidth="19725" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>categoryCode</t>
   </si>
@@ -81,6 +81,27 @@
   </si>
   <si>
     <t>001542658137</t>
+  </si>
+  <si>
+    <t>computers</t>
+  </si>
+  <si>
+    <t>electronic equipment</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>motor vehicles</t>
+  </si>
+  <si>
+    <t>computer software</t>
+  </si>
+  <si>
+    <t>land and buildings</t>
+  </si>
+  <si>
+    <t>furniture and fittings</t>
   </si>
 </sst>
 </file>
@@ -444,7 +465,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -476,9 +497,8 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="str">
-        <f>LOWER(B2)</f>
-        <v>computers</v>
+      <c r="C2" t="s">
+        <v>18</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -491,9 +511,8 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C8" si="0">LOWER(B3)</f>
-        <v>electronic equipment</v>
+      <c r="C3" t="s">
+        <v>19</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -506,9 +525,8 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>software</v>
+      <c r="C4" t="s">
+        <v>20</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -521,9 +539,8 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>motor vehicles</v>
+      <c r="C5" t="s">
+        <v>21</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -536,9 +553,8 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>computer software</v>
+      <c r="C6" t="s">
+        <v>22</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -551,9 +567,8 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="str">
-        <f>LOWER(B7)</f>
-        <v>land and buildings</v>
+      <c r="C7" t="s">
+        <v>23</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -566,9 +581,8 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>furniture and fittings</v>
+      <c r="C8" t="s">
+        <v>24</v>
       </c>
       <c r="D8">
         <v>3</v>

</xml_diff>